<commit_message>
agrego incendio para siniestros motor
</commit_message>
<xml_diff>
--- a/SuraClaims/CrearAcuerdos.xlsx
+++ b/SuraClaims/CrearAcuerdos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE3864-CB2A-4EB0-9683-8CF913524542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31CA72C-8730-47B3-B21B-5681F7578B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D2A7B85-0049-4C76-9751-BF238FCFFD27}"/>
   </bookViews>
@@ -66,13 +66,13 @@
     <t>0420194407355</t>
   </si>
   <si>
-    <t xml:space="preserve">0420194407376 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0420194407377 </t>
-  </si>
-  <si>
     <t>apellegrini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0420194407379 </t>
+  </si>
+  <si>
+    <t>0420194407380</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,13 +474,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -491,7 +491,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -508,7 +508,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -525,7 +525,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -542,7 +542,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
data para validacion generacion en SISE y para acuerdos, litigio e inspeccion
</commit_message>
<xml_diff>
--- a/SuraClaims/CrearAcuerdos.xlsx
+++ b/SuraClaims/CrearAcuerdos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B16B3A-4D05-44E1-AEC5-BFCFF616F951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE10BA2-A086-44D6-9554-6EA8E80299B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D2A7B85-0049-4C76-9751-BF238FCFFD27}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Ambiente</t>
   </si>
@@ -48,9 +48,6 @@
     <t>silverarrow</t>
   </si>
   <si>
-    <t>04104016408</t>
-  </si>
-  <si>
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
   <si>
@@ -69,22 +66,13 @@
     <t>apellegrini</t>
   </si>
   <si>
-    <t xml:space="preserve">0420194407379 </t>
-  </si>
-  <si>
-    <t>0420194407380</t>
-  </si>
-  <si>
-    <t>0420194407396</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0420194407398 </t>
-  </si>
-  <si>
     <t>0420194407400</t>
   </si>
   <si>
     <t xml:space="preserve">0420194407399 </t>
+  </si>
+  <si>
+    <t>0420172010449</t>
   </si>
 </sst>
 </file>
@@ -453,7 +441,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,75 +463,75 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,30 +542,22 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>